<commit_message>
July07 Started Explore Section: Recursion #1
P206, P344, P700
P54 NF
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D126D8E-9159-4432-ACD0-49475B2642DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924EEB49-CD1A-4C56-92C3-E60DB6C37806}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Total / Day</t>
   </si>
@@ -40,6 +40,36 @@
   </si>
   <si>
     <t>69, 125, 167, 168, 169, 70, 121, 155, 122 , M48</t>
+  </si>
+  <si>
+    <t>Explore Section (Sequence as Below)</t>
+  </si>
+  <si>
+    <t>Recursion 1</t>
+  </si>
+  <si>
+    <t>Recursion 2</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Binary Tree</t>
+  </si>
+  <si>
+    <t>Binary Search Tree</t>
+  </si>
+  <si>
+    <t>HashTable</t>
+  </si>
+  <si>
+    <t>Array and String</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Start Explore section</t>
   </si>
 </sst>
 </file>
@@ -86,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -95,6 +125,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -377,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +424,7 @@
     <col min="3" max="3" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -401,7 +435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44018</v>
       </c>
@@ -414,86 +448,121 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>44019</v>
+      </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
Recursion 2 Finished, Binary Search Started
7/11/2020, 7/12/2020		"Recursion 2 Finished, Binary Search Started: P54, P46, P94, P100, P102, P153, P162, P278, P367, P374, P658, P704, P744"
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70895EA-CBF0-4E6B-B886-5C2D8B8D8DAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F668904-BC08-4E4B-994C-B4606C1141C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="885" yWindow="1815" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Total / Day</t>
   </si>
@@ -83,7 +83,23 @@
 https://www.youtube.com/watch?v=MZaf_9IZCrc</t>
   </si>
   <si>
-    <t>P54</t>
+    <t>7/11/2020, 7/12/2020</t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>July 6 - 9</t>
+  </si>
+  <si>
+    <t>July 9 - 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 12 - </t>
+  </si>
+  <si>
+    <t>Recursion 2 Finished, Binary Search Started: P54, P46, P94, 
+P100, P102, P153, P162, P278, P367, P374, P658, P704, P744</t>
   </si>
 </sst>
 </file>
@@ -433,15 +449,16 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -507,8 +524,12 @@
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
@@ -523,8 +544,12 @@
       <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
@@ -540,13 +565,17 @@
         <v>8</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="H6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>

</xml_diff>

<commit_message>
P94, P144, P145, Recursion method & Iteration Method
P94, P144, P145, Recursion method & Iteration Method
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0008B9FE-A91E-4F82-9630-193DA8E4EBD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A9AEE-94BB-45A2-A624-64167FAA6FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1815" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="笔记" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Total / Day</t>
   </si>
@@ -107,6 +108,9 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>P94, P144, P145, Recursion method &amp; Iteration Method</t>
   </si>
 </sst>
 </file>
@@ -188,6 +192,204 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0726247-E329-48BA-8D98-0B791073FA57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="66675" y="38100"/>
+          <a:ext cx="5715000" cy="3533775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276896</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19558</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8627DCDF-CE04-44A6-ADFC-E7A959903C34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5829300" y="0"/>
+          <a:ext cx="4810796" cy="3639058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>33339</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>8667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61D83587-81CD-41F2-990B-A7BE80ACAF99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10463894" y="27214"/>
+          <a:ext cx="4877481" cy="3600953"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>435428</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>392648</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>45407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBA74036-04F0-4518-B468-018270E80502}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15131142" y="54428"/>
+          <a:ext cx="5468113" cy="3610479"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -456,7 +658,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,9 +813,13 @@
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4">
+        <v>44026</v>
+      </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
@@ -1515,4 +1721,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22318906-D15A-41F0-BEC1-17FA2B4176CB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH30" sqref="AH30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
P101, P105, P106, P112
P101, P105, P106, P112
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A9AEE-94BB-45A2-A624-64167FAA6FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458ECBF5-D344-4BF2-86DE-333DEF6BFB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Total / Day</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>P94, P144, P145, Recursion method &amp; Iteration Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 13 - </t>
+  </si>
+  <si>
+    <t>P101, P105, P106, P112</t>
   </si>
 </sst>
 </file>
@@ -658,7 +664,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,7 +800,9 @@
         <v>9</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -829,9 +837,13 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4">
+        <v>44027</v>
+      </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">

</xml_diff>

<commit_message>
P116, P117, P236, Binary Tree finished only one HARD question P297 Left P173, Binary Search Tree(BST) started, P700 Iteration Method Implemented
P116, P117, P236, Binary Tree finished only one HARD question P297 Left
P173, Binary Search Tree(BST) started, P700 Iteration Method Implemented
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458ECBF5-D344-4BF2-86DE-333DEF6BFB38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B05F170-B696-462A-90C9-8178A5B0347E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Total / Day</t>
   </si>
@@ -113,10 +113,17 @@
     <t>P94, P144, P145, Recursion method &amp; Iteration Method</t>
   </si>
   <si>
-    <t xml:space="preserve">July 13 - </t>
-  </si>
-  <si>
     <t>P101, P105, P106, P112</t>
+  </si>
+  <si>
+    <t>July 13 - July 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 16 - </t>
+  </si>
+  <si>
+    <t>P116, P117, P236, Binary Tree finished only one HARD question P297 Left
+P173, Binary Search Tree(BST) started, P700 Iteration Method Implemented</t>
   </si>
 </sst>
 </file>
@@ -163,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,6 +189,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,14 +674,14 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="65.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -799,9 +809,11 @@
       <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="H7" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -818,7 +830,9 @@
         <v>10</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -842,7 +856,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -852,10 +866,14 @@
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44028</v>
+      </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">

</xml_diff>

<commit_message>
P450, P701, P220, P235, P703 220: TreeSet; 703: PriorityQueue
P450, P701, P220, P235, P703
220: TreeSet; 703: PriorityQueue
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B05F170-B696-462A-90C9-8178A5B0347E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321D9E9-3FDD-466B-9B5A-4FFDDC0FE7A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Total / Day</t>
   </si>
@@ -124,6 +124,13 @@
   <si>
     <t>P116, P117, P236, Binary Tree finished only one HARD question P297 Left
 P173, Binary Search Tree(BST) started, P700 Iteration Method Implemented</t>
+  </si>
+  <si>
+    <t>7/17/2020, 7/15/2020</t>
+  </si>
+  <si>
+    <t>P450, P701, P220, P235, P703
+220: TreeSet; 703: PriorityQueue</t>
   </si>
 </sst>
 </file>
@@ -674,7 +681,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,10 +889,14 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>

</xml_diff>

<commit_message>
P108, 110, 202, 205, 217, 219, 387, 599, 705, 706
P108, 110, 202, 205, 217, 219, 387, 599, 705, 706
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8321D9E9-3FDD-466B-9B5A-4FFDDC0FE7A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA05826-686C-4166-92EF-4E4C8726C0F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="2355" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Total / Day</t>
   </si>
@@ -107,9 +107,6 @@
     <t>July 6 - July 9</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>P94, P144, P145, Recursion method &amp; Iteration Method</t>
   </si>
   <si>
@@ -117,20 +114,26 @@
   </si>
   <si>
     <t>July 13 - July 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">July 16 - </t>
   </si>
   <si>
     <t>P116, P117, P236, Binary Tree finished only one HARD question P297 Left
 P173, Binary Search Tree(BST) started, P700 Iteration Method Implemented</t>
   </si>
   <si>
-    <t>7/17/2020, 7/15/2020</t>
-  </si>
-  <si>
-    <t>P450, P701, P220, P235, P703
+    <t>(First 100 Questions) P450, P701, P220, P235, P703
 220: TreeSet; 703: PriorityQueue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 16 - July 19 </t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>7/17/2020, 7/18/2020</t>
+  </si>
+  <si>
+    <t>P108, 110, 202, 205, 217, 219, 387, 599, 705, 706</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +155,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -198,6 +207,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -681,7 +693,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +809,7 @@
         <v>8</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>22</v>
@@ -817,10 +829,10 @@
         <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -836,9 +848,11 @@
       <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H8" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -847,15 +861,19 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="7">
+        <v>44031</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
@@ -863,7 +881,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -879,7 +897,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -891,11 +909,11 @@
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -904,9 +922,13 @@
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4">
+        <v>44031</v>
+      </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1759,6 +1781,7 @@
       <c r="D168" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
P49, P454, P652, P771, Review P3
P49, P454, P652, P771, Review P3
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA05826-686C-4166-92EF-4E4C8726C0F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AE491-0661-4B03-9F79-2F643B7D1990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2355" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Total / Day</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>P108, 110, 202, 205, 217, 219, 387, 599, 705, 706</t>
+  </si>
+  <si>
+    <t>P49, P454, P652, P771, Review P3</t>
+  </si>
+  <si>
+    <t>Cook</t>
   </si>
 </sst>
 </file>
@@ -693,7 +699,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,11 +942,17 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4">
+        <v>44032</v>
+      </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>

</xml_diff>

<commit_message>
"P118, P347, P380, P498, P724, P747 HashTable finished, Array and String Started"
"P118, P347, P380, P498, P724, P747
HashTable finished, Array and String Started"
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877AE491-0661-4B03-9F79-2F643B7D1990}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBDF158-10CE-4624-8308-B4CA78254970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,28 +16,28 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="笔记" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Total / Day</t>
   </si>
   <si>
     <t>Details</t>
-  </si>
-  <si>
-    <t>Difficulty</t>
-  </si>
-  <si>
-    <t>E</t>
   </si>
   <si>
     <t>69, 125, 167, 168, 169, 70, 121, 155, 122 , M48</t>
@@ -127,9 +127,6 @@
     <t xml:space="preserve">July 16 - July 19 </t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>7/17/2020, 7/18/2020</t>
   </si>
   <si>
@@ -140,6 +137,22 @@
   </si>
   <si>
     <t>Cook</t>
+  </si>
+  <si>
+    <t>Jogging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 19 - July 21 </t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 21 - July  </t>
+  </si>
+  <si>
+    <t>P118, P347, P380, P498, P724, P747
+HashTable finished, Array and String Started</t>
   </si>
 </sst>
 </file>
@@ -699,7 +712,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,8 +732,9 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
+      <c r="D1" s="3">
+        <f>SUM(D2:D15)</f>
+        <v>80</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -735,10 +749,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>10</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -751,12 +765,12 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -767,18 +781,20 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -787,18 +803,20 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -807,38 +825,42 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="D6" s="5">
+        <v>3</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="D7" s="5">
+        <v>13</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -847,18 +869,20 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -867,18 +891,20 @@
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="7">
-        <v>44031</v>
+        <v>35</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -887,15 +913,19 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="H10" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -903,25 +933,29 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7</v>
+      </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -933,9 +967,11 @@
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="D13" s="5">
+        <v>10</v>
+      </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -947,22 +983,32 @@
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>44033</v>
+      </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>

</xml_diff>

<commit_message>
P27, P151, P189, P209, P485
P27, P151, P189, P209, P485
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBDF158-10CE-4624-8308-B4CA78254970}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B5585-FFEE-47C4-A5CC-41BD70068387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Total / Day</t>
   </si>
@@ -153,6 +153,9 @@
   <si>
     <t>P118, P347, P380, P498, P724, P747
 HashTable finished, Array and String Started</t>
+  </si>
+  <si>
+    <t>P27, P151, P189, P209, P485</t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,11 +1017,19 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4">
+        <v>44034</v>
+      </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>

</xml_diff>

<commit_message>
P283, P557, P707 NG
P283, P557, P707 NG
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01B5585-FFEE-47C4-A5CC-41BD70068387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47A505F-338A-4C8E-9265-68305A7ABFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Total / Day</t>
   </si>
@@ -148,14 +148,17 @@
     <t>Check</t>
   </si>
   <si>
-    <t xml:space="preserve">July 21 - July  </t>
-  </si>
-  <si>
     <t>P118, P347, P380, P498, P724, P747
 HashTable finished, Array and String Started</t>
   </si>
   <si>
     <t>P27, P151, P189, P209, P485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 21 - July 23 </t>
+  </si>
+  <si>
+    <t>P283, P557, P707 NG</t>
   </si>
 </sst>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,8 +739,8 @@
         <v>1</v>
       </c>
       <c r="D1" s="3">
-        <f>SUM(D2:D15)</f>
-        <v>80</v>
+        <f>SUM(D2:D157)</f>
+        <v>88</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -925,9 +928,11 @@
       <c r="F10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="H10" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1004,7 +1009,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="5">
         <v>6</v>
@@ -1022,7 +1027,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" s="5">
         <v>5</v>
@@ -1035,10 +1040,16 @@
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4">
+        <v>44035</v>
+      </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>

</xml_diff>

<commit_message>
P142, P160, P203, P234, P328
P142, P160, P203, P234, P328
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47A505F-338A-4C8E-9265-68305A7ABFC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232F4683-165C-428C-B8B8-EDE837221FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5385" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Total / Day</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>P283, P557, P707 NG</t>
+  </si>
+  <si>
+    <t>P142, P160, P203, P234, P328</t>
   </si>
 </sst>
 </file>
@@ -718,7 +721,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +743,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1056,10 +1059,16 @@
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4">
+        <v>44036</v>
+      </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>

</xml_diff>

<commit_message>
P61, P138, P200, P429, P430, P559, P589, P590, P622, P752
P61, P138, P200, P429, P430, P559, P589, P590, P622, P752
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232F4683-165C-428C-B8B8-EDE837221FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915FBD28-C826-41DB-BCBE-09449F5AEC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="2100" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="2475" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Total / Day</t>
   </si>
@@ -145,9 +145,6 @@
     <t xml:space="preserve">July 19 - July 21 </t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>P118, P347, P380, P498, P724, P747
 HashTable finished, Array and String Started</t>
   </si>
@@ -162,6 +159,33 @@
   </si>
   <si>
     <t>P142, P160, P203, P234, P328</t>
+  </si>
+  <si>
+    <t>7/25/2020, 7/26/2020</t>
+  </si>
+  <si>
+    <t>July 23 - July 26</t>
+  </si>
+  <si>
+    <t>N-ary Tree</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>July 26 - July 26</t>
+  </si>
+  <si>
+    <t>Queue &amp; Stack</t>
+  </si>
+  <si>
+    <t>July 26 -</t>
+  </si>
+  <si>
+    <t>Anniversay, Cook</t>
+  </si>
+  <si>
+    <t>P61, P138, P200, P429, P430, P559, P589, P590, P622, P752</t>
   </si>
 </sst>
 </file>
@@ -452,6 +476,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>81644</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>469167</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>136869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0598A5F3-DC0D-4344-ADF8-22ACE307DEB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="81644" y="3755571"/>
+          <a:ext cx="7735380" cy="5715798"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -720,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +797,8 @@
     <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
     <col min="3" max="3" width="70.5703125" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -743,7 +812,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -910,7 +979,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>34</v>
@@ -935,7 +1004,7 @@
         <v>17</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -953,8 +1022,12 @@
       <c r="F11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -968,9 +1041,15 @@
         <v>7</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -984,9 +1063,13 @@
         <v>10</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
@@ -1012,7 +1095,7 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="5">
         <v>6</v>
@@ -1030,7 +1113,7 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5">
         <v>5</v>
@@ -1048,7 +1131,7 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="5">
         <v>3</v>
@@ -1064,7 +1147,7 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="5">
         <v>5</v>
@@ -1075,11 +1158,19 @@
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="5">
+        <v>10</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1880,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22318906-D15A-41F0-BEC1-17FA2B4176CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH30" sqref="AH30"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
P133, P150, P225, P232, P279, P494, P739
P133, P150, P225, P232, P279, P494, P739
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915FBD28-C826-41DB-BCBE-09449F5AEC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DD17AA-F233-4E18-80D7-511BEDCCD5AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="2475" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2775" yWindow="2430" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="笔记" sheetId="2" r:id="rId2"/>
+    <sheet name="一刷看答案" sheetId="3" r:id="rId2"/>
+    <sheet name="笔记" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Total / Day</t>
   </si>
@@ -186,6 +187,9 @@
   </si>
   <si>
     <t>P61, P138, P200, P429, P430, P559, P589, P590, P622, P752</t>
+  </si>
+  <si>
+    <t>P133, P150, P225, P232, P279, P494, P739</t>
   </si>
 </sst>
 </file>
@@ -238,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,6 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -788,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,7 +817,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1176,10 +1181,16 @@
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4">
+        <v>44039</v>
+      </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="5">
+        <v>7</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1968,10 +1979,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ABA50E-0128-4FDD-A4EC-1CCC7866BDAC}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="9">
+        <v>44039</v>
+      </c>
+      <c r="B1">
+        <v>133</v>
+      </c>
+      <c r="C1">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22318906-D15A-41F0-BEC1-17FA2B4176CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
P394, P542, P733, P841, P43
P394, P542, P733, P841, P43
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DD17AA-F233-4E18-80D7-511BEDCCD5AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E076852-AC77-49CA-A4C0-C29247DC68A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2775" yWindow="2430" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Total / Day</t>
   </si>
@@ -171,18 +171,12 @@
     <t>N-ary Tree</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
     <t>July 26 - July 26</t>
   </si>
   <si>
     <t>Queue &amp; Stack</t>
   </si>
   <si>
-    <t>July 26 -</t>
-  </si>
-  <si>
     <t>Anniversay, Cook</t>
   </si>
   <si>
@@ -190,6 +184,18 @@
   </si>
   <si>
     <t>P133, P150, P225, P232, P279, P494, P739</t>
+  </si>
+  <si>
+    <t>July 26 - July 28</t>
+  </si>
+  <si>
+    <t>Array 101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 29 - July </t>
+  </si>
+  <si>
+    <t>P394, P542, P733, P841, P43</t>
   </si>
 </sst>
 </file>
@@ -794,7 +800,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,7 +823,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1050,10 +1056,10 @@
         <v>42</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1069,11 +1075,13 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="H13" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1090,9 +1098,13 @@
       <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1168,13 +1180,13 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5">
         <v>10</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1186,7 +1198,7 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="5">
         <v>7</v>
@@ -1197,11 +1209,19 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4">
+        <v>44040</v>
+      </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1980,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ABA50E-0128-4FDD-A4EC-1CCC7866BDAC}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +2011,7 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9">
         <v>44039</v>
       </c>
@@ -2000,6 +2020,28 @@
       </c>
       <c r="C1">
         <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>44040</v>
+      </c>
+      <c r="B2">
+        <v>394</v>
+      </c>
+      <c r="C2">
+        <v>733</v>
+      </c>
+      <c r="D2">
+        <v>841</v>
+      </c>
+      <c r="E2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>44041</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22318906-D15A-41F0-BEC1-17FA2B4176CB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Y32" sqref="Y32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
P977, P1089, P1295, P1346
P977, P1089, P1295, P1346
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E076852-AC77-49CA-A4C0-C29247DC68A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7B6210-FB03-4747-BD60-CD54D3F1DE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2430" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="2385" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>Total / Day</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>P394, P542, P733, P841, P43</t>
+  </si>
+  <si>
+    <t>Costco</t>
+  </si>
+  <si>
+    <t>P977, P1089, P1295, P1346</t>
   </si>
 </sst>
 </file>
@@ -800,7 +806,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +829,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1217,7 +1223,7 @@
         <v>51</v>
       </c>
       <c r="D21" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>32</v>
@@ -1227,11 +1233,19 @@
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4">
+        <v>44041</v>
+      </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="5">
+        <v>4</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>

</xml_diff>

<commit_message>
P47, P414, P448, P905, P941, P1051, P1299
P47, P414, P448, P905, P941, P1051, P1299
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7B6210-FB03-4747-BD60-CD54D3F1DE8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B540A31D-D06B-4519-AF22-0D0A64487F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5130" yWindow="2385" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Total / Day</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Array 101</t>
   </si>
   <si>
-    <t xml:space="preserve">July 29 - July </t>
-  </si>
-  <si>
     <t>P394, P542, P733, P841, P43</t>
   </si>
   <si>
@@ -202,6 +199,12 @@
   </si>
   <si>
     <t>P977, P1089, P1295, P1346</t>
+  </si>
+  <si>
+    <t>July 29 - July  30</t>
+  </si>
+  <si>
+    <t>P47, P414, P448, P905, P941, P1051, P1299</t>
   </si>
 </sst>
 </file>
@@ -805,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +832,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1107,9 +1110,11 @@
       <c r="F14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="H14" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1220,7 +1225,7 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="5">
         <v>5</v>
@@ -1238,23 +1243,29 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="5">
         <v>4</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="4">
+        <v>44042</v>
+      </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="5">
+        <v>7</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -2014,10 +2025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ABA50E-0128-4FDD-A4EC-1CCC7866BDAC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,6 +2067,14 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>44041</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>44042</v>
+      </c>
+      <c r="B4">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
P55, P56, P109, P113, P114, P129
P55, P56, P109, P113, P114, P129
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B540A31D-D06B-4519-AF22-0D0A64487F5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77161996-4F7F-4150-9067-08C8BD3309E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5130" yWindow="2385" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Total / Day</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>P47, P414, P448, P905, P941, P1051, P1299</t>
+  </si>
+  <si>
+    <t>P55, P56, P109, P113, P114, P129</t>
   </si>
 </sst>
 </file>
@@ -808,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +835,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1272,10 +1275,16 @@
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4">
+        <v>44043</v>
+      </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="5">
+        <v>6</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -2025,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ABA50E-0128-4FDD-A4EC-1CCC7866BDAC}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,6 +2084,17 @@
       </c>
       <c r="B4">
         <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>44043</v>
+      </c>
+      <c r="B5">
+        <v>109</v>
+      </c>
+      <c r="C5">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
P130, P59, P62(DP思想), P63, P64, P71(split), P73, P74, P107, P111, P75,P78
P130, P59, P62(DP思想), P63, P64, P71(split), P73, P74, P107, P111, P75,P78
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77161996-4F7F-4150-9067-08C8BD3309E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEB38BB-2D25-4478-A403-8E65C58EC231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="2385" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5475" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Total / Day</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>P55, P56, P109, P113, P114, P129</t>
+  </si>
+  <si>
+    <t>P130, P59, P62(DP思想), P63, P64, P71(split), P73, P74, P107, P111, P75,P78</t>
   </si>
 </sst>
 </file>
@@ -812,7 +815,7 @@
   <dimension ref="A1:H168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +838,7 @@
       </c>
       <c r="D1" s="3">
         <f>SUM(D2:D157)</f>
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1291,10 +1294,16 @@
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="4">
+        <v>44044</v>
+      </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -2034,10 +2043,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ABA50E-0128-4FDD-A4EC-1CCC7866BDAC}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,6 +2104,23 @@
       </c>
       <c r="C5">
         <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>44044</v>
+      </c>
+      <c r="B6">
+        <v>130</v>
+      </c>
+      <c r="C6">
+        <v>62</v>
+      </c>
+      <c r="D6">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
P79(更简约的DFS), P80, P81, P82, P86, P89(格雷码有固定公式), P90, P91(DP 重点)
P79(更简约的DFS), P80, P81, P82, P86, P89(格雷码有固定公式), P90, P91(DP 重点)
</commit_message>
<xml_diff>
--- a/Log_LeetCode.xlsx
+++ b/Log_LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shado\Desktop\Work_Space\LeetCode_JJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEB38BB-2D25-4478-A403-8E65C58EC231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF532AE-9427-44E4-B189-DB8C6DCD26F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5475" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>